<commit_message>
usuario tambien puede ser profesor
</commit_message>
<xml_diff>
--- a/public/Equipos_Docentes.xlsx
+++ b/public/Equipos_Docentes.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$150</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="198">
   <si>
     <t>CODIGO</t>
   </si>
@@ -1079,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>19</v>
@@ -1580,9 +1580,7 @@
       <c r="D38" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>195</v>
-      </c>
+      <c r="E38" s="7"/>
       <c r="F38" s="7" t="s">
         <v>115</v>
       </c>
@@ -1594,15 +1592,13 @@
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="6">
-        <v>2</v>
-      </c>
+      <c r="C40" s="6"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7" t="s">
@@ -1616,25 +1612,19 @@
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="A42" s="4"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="6">
-        <v>1</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>177</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,7 +1634,7 @@
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1654,7 +1644,7 @@
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1664,7 +1654,7 @@
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7" t="s">
-        <v>180</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1674,14 +1664,18 @@
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="7"/>
+      <c r="A47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C47" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>177</v>
@@ -1714,7 +1708,7 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="6"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7" t="s">
@@ -1732,219 +1726,211 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="A52" s="4"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>143</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E52" s="7"/>
       <c r="F52" s="7" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
       <c r="C53" s="6"/>
-      <c r="D53" s="7" t="s">
-        <v>140</v>
-      </c>
+      <c r="D53" s="7"/>
       <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
+      <c r="F53" s="7" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="7"/>
-      <c r="C54" s="6">
-        <v>2</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>145</v>
-      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="7"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7" t="s">
-        <v>144</v>
-      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
       <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
+      <c r="F55" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="7"/>
-      <c r="C56" s="6">
-        <v>3</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7" t="s">
-        <v>147</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="6"/>
+      <c r="A57" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="6">
+        <v>1</v>
+      </c>
       <c r="D57" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+        <v>141</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="7"/>
-      <c r="C58" s="6">
-        <v>4</v>
-      </c>
+      <c r="C58" s="6"/>
       <c r="D58" s="7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E58" s="7"/>
-      <c r="F58" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="7"/>
-      <c r="C59" s="6"/>
+      <c r="C59" s="6">
+        <v>2</v>
+      </c>
       <c r="D59" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
+      <c r="F59" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="7"/>
-      <c r="C60" s="6">
-        <v>5</v>
-      </c>
+      <c r="C60" s="6"/>
       <c r="D60" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E60" s="7"/>
-      <c r="F60" s="7" t="s">
-        <v>153</v>
-      </c>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="7"/>
-      <c r="C61" s="6"/>
+      <c r="C61" s="6">
+        <v>3</v>
+      </c>
       <c r="D61" s="7" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
+      <c r="F61" s="7" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="6">
-        <v>1</v>
-      </c>
+      <c r="A62" s="4"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="6"/>
       <c r="D62" s="7" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="E62" s="7"/>
-      <c r="F62" s="7" t="s">
-        <v>184</v>
-      </c>
+      <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="7"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="7"/>
+      <c r="C63" s="6">
+        <v>4</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="7"/>
       <c r="C64" s="6"/>
-      <c r="D64" s="7"/>
+      <c r="D64" s="7" t="s">
+        <v>148</v>
+      </c>
       <c r="E64" s="7"/>
-      <c r="F64" s="7" t="s">
-        <v>183</v>
-      </c>
+      <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="7"/>
       <c r="C65" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="7"/>
       <c r="C66" s="6"/>
-      <c r="D66" s="7"/>
+      <c r="D66" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="E66" s="7"/>
-      <c r="F66" s="7" t="s">
-        <v>182</v>
-      </c>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="7"/>
+      <c r="A67" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="6">
+        <v>1</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="6">
-        <v>1</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="A68" s="4"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1954,119 +1940,111 @@
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="7"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="7"/>
+      <c r="C70" s="6">
+        <v>2</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="6">
-        <v>1</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>120</v>
-      </c>
+      <c r="A71" s="4"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
       <c r="F71" s="7" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="7"/>
       <c r="C72" s="6"/>
-      <c r="D72" s="7" t="s">
-        <v>118</v>
-      </c>
+      <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7" t="s">
-        <v>58</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="7"/>
+      <c r="A73" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="6">
+        <v>1</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="7"/>
-      <c r="C74" s="6">
-        <v>2</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>119</v>
-      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="7"/>
       <c r="E74" s="7"/>
-      <c r="F74" s="9"/>
+      <c r="F74" s="7" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="7"/>
       <c r="C75" s="6"/>
-      <c r="D75" s="7" t="s">
-        <v>118</v>
-      </c>
+      <c r="D75" s="7"/>
       <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
+      <c r="F75" s="7" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C76" s="6">
         <v>1</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E76" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="F76" s="7" t="s">
-        <v>186</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C77" s="6">
-        <v>1</v>
-      </c>
+      <c r="A77" s="4"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="6"/>
       <c r="D77" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>126</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E77" s="7"/>
       <c r="F77" s="7" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2076,7 +2054,7 @@
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2086,101 +2064,111 @@
         <v>2</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E79" s="7"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C80" s="6">
+      <c r="A80" s="4"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C81" s="6">
         <v>1</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="6"/>
       <c r="D81" s="7" t="s">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="E81" s="7"/>
       <c r="F81" s="7" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
+      <c r="A82" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" s="6">
+        <v>1</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="F82" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="7"/>
-      <c r="C83" s="6">
+      <c r="C83" s="6"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="6">
         <v>2</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E83" s="7"/>
-      <c r="F83" s="9"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C84" s="6">
+      <c r="D84" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E84" s="7"/>
+      <c r="F84" s="9"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="6">
         <v>1</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
+      <c r="D85" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="F85" s="7" t="s">
-        <v>197</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="7"/>
       <c r="C86" s="6"/>
-      <c r="D86" s="7"/>
+      <c r="D86" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="E86" s="7"/>
       <c r="F86" s="7" t="s">
-        <v>188</v>
+        <v>129</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2190,312 +2178,310 @@
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
+      <c r="C88" s="6">
+        <v>2</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>133</v>
+      </c>
       <c r="E88" s="7"/>
-      <c r="F88" s="7" t="s">
-        <v>189</v>
-      </c>
+      <c r="F88" s="9"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="7"/>
+      <c r="A89" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C89" s="6">
+        <v>1</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>187</v>
+      </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7" t="s">
-        <v>190</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
+      <c r="C90" s="6"/>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
-      <c r="F90" s="13" t="s">
-        <v>121</v>
+      <c r="F90" s="7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
+      <c r="C91" s="6"/>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
-      <c r="F91" s="13" t="s">
-        <v>167</v>
+      <c r="F91" s="7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C92" s="6">
-        <v>1</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
       <c r="F92" s="7" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="7"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
       <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
+      <c r="F93" s="7" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="7"/>
-      <c r="C94" s="6">
-        <v>2</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>157</v>
-      </c>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
       <c r="E94" s="7"/>
-      <c r="F94" s="10" t="s">
-        <v>81</v>
+      <c r="F94" s="7" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C95" s="6">
-        <v>1</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A95" s="4"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
       <c r="E95" s="7"/>
-      <c r="F95" s="7" t="s">
-        <v>57</v>
+      <c r="F95" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="7"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
       <c r="E96" s="7"/>
-      <c r="F96" s="7" t="s">
-        <v>196</v>
+      <c r="F96" s="13" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
+      <c r="A97" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="F97" s="7" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C98" s="6">
-        <v>1</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>191</v>
+      <c r="A98" s="4"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="E98" s="7"/>
-      <c r="F98" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="F98" s="7"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="7"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="7"/>
+      <c r="C99" s="6">
+        <v>2</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>157</v>
+      </c>
       <c r="E99" s="7"/>
-      <c r="F99" s="7" t="s">
-        <v>169</v>
+      <c r="F99" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C100" s="6">
         <v>1</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>192</v>
+        <v>56</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="7"/>
       <c r="C101" s="6"/>
-      <c r="D101" s="7"/>
+      <c r="D101" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C102" s="6">
+      <c r="A102" s="4"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C103" s="6">
         <v>1</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="6">
-        <v>2</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>161</v>
+      <c r="D103" s="14" t="s">
+        <v>191</v>
       </c>
       <c r="E103" s="7"/>
-      <c r="F103" s="7"/>
+      <c r="F103" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C104" s="6">
+      <c r="A104" s="4"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C105" s="6">
         <v>1</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E104" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="7"/>
+      <c r="D105" s="7" t="s">
+        <v>192</v>
+      </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="7"/>
-      <c r="C106" s="6">
-        <v>2</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>134</v>
-      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
+      <c r="A107" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C107" s="6">
+        <v>1</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="F107" s="7" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="7"/>
+      <c r="C108" s="6">
+        <v>2</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="E108" s="7"/>
-      <c r="F108" s="7" t="s">
-        <v>139</v>
-      </c>
+      <c r="F108" s="7"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C109" s="6">
         <v>1</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E109" s="7"/>
+        <v>134</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="F109" s="7" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="7"/>
       <c r="C110" s="6"/>
-      <c r="D110" s="7" t="s">
-        <v>162</v>
-      </c>
+      <c r="D110" s="7"/>
       <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
+      <c r="F110" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
@@ -2504,67 +2490,69 @@
         <v>2</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
+      <c r="F111" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="7"/>
       <c r="C112" s="6"/>
-      <c r="D112" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="D112" s="7"/>
       <c r="E112" s="7"/>
-      <c r="F112" s="7"/>
+      <c r="F112" s="7" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="7"/>
-      <c r="C113" s="6">
-        <v>3</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>166</v>
-      </c>
+      <c r="C113" s="6"/>
+      <c r="D113" s="7"/>
       <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
+      <c r="F113" s="7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="4"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="6"/>
+      <c r="A114" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114" s="6">
+        <v>1</v>
+      </c>
       <c r="D114" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
+      <c r="F114" s="7" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C115" s="6">
-        <v>1</v>
-      </c>
+      <c r="A115" s="4"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="6"/>
       <c r="D115" s="7" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="E115" s="7"/>
-      <c r="F115" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F115" s="7"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="7"/>
-      <c r="C116" s="6"/>
+      <c r="C116" s="6">
+        <v>2</v>
+      </c>
       <c r="D116" s="7" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
@@ -2574,7 +2562,7 @@
       <c r="B117" s="7"/>
       <c r="C117" s="6"/>
       <c r="D117" s="7" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
@@ -2583,56 +2571,58 @@
       <c r="A118" s="4"/>
       <c r="B118" s="7"/>
       <c r="C118" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="E118" s="7"/>
-      <c r="F118" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F118" s="7"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="7"/>
       <c r="C119" s="6"/>
       <c r="D119" s="7" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="12"/>
-      <c r="D120" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E120" s="5"/>
-      <c r="F120" s="11"/>
+      <c r="A120" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C120" s="6">
+        <v>1</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E120" s="7"/>
+      <c r="F120" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="7"/>
-      <c r="C121" s="6">
-        <v>3</v>
-      </c>
+      <c r="C121" s="6"/>
       <c r="D121" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E121" s="7"/>
-      <c r="F121" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F121" s="7"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="7"/>
       <c r="C122" s="6"/>
       <c r="D122" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E122" s="7"/>
       <c r="F122" s="7"/>
@@ -2640,67 +2630,67 @@
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="7"/>
-      <c r="C123" s="6"/>
+      <c r="C123" s="6">
+        <v>2</v>
+      </c>
       <c r="D123" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
+      <c r="F123" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="7"/>
-      <c r="C124" s="6">
-        <v>4</v>
-      </c>
+      <c r="C124" s="6"/>
       <c r="D124" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E124" s="7"/>
-      <c r="F124" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F124" s="7"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="6"/>
-      <c r="D125" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E125" s="7"/>
-      <c r="F125" s="7"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E125" s="5"/>
+      <c r="F125" s="11"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="7"/>
-      <c r="C126" s="6"/>
+      <c r="C126" s="6">
+        <v>3</v>
+      </c>
       <c r="D126" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E126" s="7"/>
-      <c r="F126" s="7"/>
+      <c r="F126" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="7"/>
-      <c r="C127" s="6">
-        <v>5</v>
-      </c>
+      <c r="C127" s="6"/>
       <c r="D127" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E127" s="7"/>
-      <c r="F127" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F127" s="7"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="7"/>
       <c r="C128" s="6"/>
       <c r="D128" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
@@ -2708,33 +2698,33 @@
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="7"/>
-      <c r="C129" s="6"/>
+      <c r="C129" s="6">
+        <v>4</v>
+      </c>
       <c r="D129" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E129" s="7"/>
-      <c r="F129" s="7"/>
+      <c r="F129" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="7"/>
-      <c r="C130" s="6">
-        <v>6</v>
-      </c>
+      <c r="C130" s="6"/>
       <c r="D130" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E130" s="7"/>
-      <c r="F130" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F130" s="7"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="7"/>
       <c r="C131" s="6"/>
       <c r="D131" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
@@ -2742,33 +2732,33 @@
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="7"/>
-      <c r="C132" s="6"/>
+      <c r="C132" s="6">
+        <v>5</v>
+      </c>
       <c r="D132" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
+      <c r="F132" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="7"/>
-      <c r="C133" s="6">
-        <v>7</v>
-      </c>
+      <c r="C133" s="6"/>
       <c r="D133" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E133" s="7"/>
-      <c r="F133" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F133" s="7"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="7"/>
       <c r="C134" s="6"/>
       <c r="D134" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E134" s="7"/>
       <c r="F134" s="7"/>
@@ -2776,33 +2766,33 @@
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" s="7"/>
-      <c r="C135" s="6"/>
+      <c r="C135" s="6">
+        <v>6</v>
+      </c>
       <c r="D135" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E135" s="7"/>
-      <c r="F135" s="7"/>
+      <c r="F135" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" s="7"/>
-      <c r="C136" s="6">
-        <v>8</v>
-      </c>
+      <c r="C136" s="6"/>
       <c r="D136" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E136" s="7"/>
-      <c r="F136" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F136" s="7"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="7"/>
       <c r="C137" s="6"/>
       <c r="D137" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
@@ -2810,33 +2800,33 @@
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
       <c r="B138" s="7"/>
-      <c r="C138" s="6"/>
+      <c r="C138" s="6">
+        <v>7</v>
+      </c>
       <c r="D138" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
+      <c r="F138" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="7"/>
-      <c r="C139" s="6">
-        <v>9</v>
-      </c>
+      <c r="C139" s="6"/>
       <c r="D139" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E139" s="7"/>
-      <c r="F139" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F139" s="7"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="7"/>
       <c r="C140" s="6"/>
       <c r="D140" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E140" s="7"/>
       <c r="F140" s="7"/>
@@ -2844,33 +2834,33 @@
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="7"/>
-      <c r="C141" s="6"/>
+      <c r="C141" s="6">
+        <v>8</v>
+      </c>
       <c r="D141" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
+      <c r="F141" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="7"/>
-      <c r="C142" s="6">
-        <v>10</v>
-      </c>
+      <c r="C142" s="6"/>
       <c r="D142" s="7" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="E142" s="7"/>
-      <c r="F142" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F142" s="7"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="7"/>
       <c r="C143" s="6"/>
       <c r="D143" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E143" s="7"/>
       <c r="F143" s="7"/>
@@ -2878,59 +2868,57 @@
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="7"/>
-      <c r="C144" s="6"/>
+      <c r="C144" s="6">
+        <v>9</v>
+      </c>
       <c r="D144" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
+      <c r="F144" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
       <c r="B145" s="7"/>
-      <c r="C145" s="6">
-        <v>11</v>
-      </c>
+      <c r="C145" s="6"/>
       <c r="D145" s="7" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="7"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C146" s="6">
-        <v>1</v>
-      </c>
+      <c r="A146" s="4"/>
+      <c r="B146" s="7"/>
+      <c r="C146" s="6"/>
       <c r="D146" s="7" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E146" s="7"/>
-      <c r="F146" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F146" s="7"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="4"/>
       <c r="B147" s="7"/>
-      <c r="C147" s="6"/>
+      <c r="C147" s="6">
+        <v>10</v>
+      </c>
       <c r="D147" s="7" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
+      <c r="F147" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
       <c r="B148" s="7"/>
       <c r="C148" s="6"/>
       <c r="D148" s="7" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="E148" s="7"/>
       <c r="F148" s="7"/>
@@ -2938,57 +2926,59 @@
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
       <c r="B149" s="7"/>
-      <c r="C149" s="6">
-        <v>2</v>
-      </c>
+      <c r="C149" s="6"/>
       <c r="D149" s="7" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="E149" s="7"/>
-      <c r="F149" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F149" s="7"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="4"/>
       <c r="B150" s="7"/>
-      <c r="C150" s="6"/>
+      <c r="C150" s="6">
+        <v>11</v>
+      </c>
       <c r="D150" s="7" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E150" s="7"/>
       <c r="F150" s="7"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
-      <c r="B151" s="11"/>
-      <c r="C151" s="12"/>
-      <c r="D151" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E151" s="5"/>
-      <c r="F151" s="11"/>
+      <c r="A151" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C151" s="6">
+        <v>1</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E151" s="7"/>
+      <c r="F151" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="4"/>
       <c r="B152" s="7"/>
-      <c r="C152" s="6">
-        <v>3</v>
-      </c>
+      <c r="C152" s="6"/>
       <c r="D152" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E152" s="7"/>
-      <c r="F152" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F152" s="7"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="7"/>
       <c r="C153" s="6"/>
       <c r="D153" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
@@ -2996,67 +2986,67 @@
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
       <c r="B154" s="7"/>
-      <c r="C154" s="6"/>
+      <c r="C154" s="6">
+        <v>2</v>
+      </c>
       <c r="D154" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
+      <c r="F154" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="7"/>
-      <c r="C155" s="6">
-        <v>4</v>
-      </c>
+      <c r="C155" s="6"/>
       <c r="D155" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E155" s="7"/>
-      <c r="F155" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F155" s="7"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
-      <c r="B156" s="7"/>
-      <c r="C156" s="6"/>
-      <c r="D156" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E156" s="7"/>
-      <c r="F156" s="7"/>
+      <c r="B156" s="11"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E156" s="5"/>
+      <c r="F156" s="11"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="7"/>
-      <c r="C157" s="6"/>
+      <c r="C157" s="6">
+        <v>3</v>
+      </c>
       <c r="D157" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E157" s="7"/>
-      <c r="F157" s="7"/>
+      <c r="F157" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="7"/>
-      <c r="C158" s="6">
-        <v>5</v>
-      </c>
+      <c r="C158" s="6"/>
       <c r="D158" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E158" s="7"/>
-      <c r="F158" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F158" s="7"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="7"/>
       <c r="C159" s="6"/>
       <c r="D159" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
@@ -3064,33 +3054,33 @@
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="7"/>
-      <c r="C160" s="6"/>
+      <c r="C160" s="6">
+        <v>4</v>
+      </c>
       <c r="D160" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
+      <c r="F160" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="7"/>
-      <c r="C161" s="6">
-        <v>6</v>
-      </c>
+      <c r="C161" s="6"/>
       <c r="D161" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E161" s="7"/>
-      <c r="F161" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F161" s="7"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="7"/>
       <c r="C162" s="6"/>
       <c r="D162" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
@@ -3098,33 +3088,33 @@
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="7"/>
-      <c r="C163" s="6"/>
+      <c r="C163" s="6">
+        <v>5</v>
+      </c>
       <c r="D163" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
+      <c r="F163" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="7"/>
-      <c r="C164" s="6">
-        <v>7</v>
-      </c>
+      <c r="C164" s="6"/>
       <c r="D164" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E164" s="7"/>
-      <c r="F164" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F164" s="7"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="7"/>
       <c r="C165" s="6"/>
       <c r="D165" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E165" s="7"/>
       <c r="F165" s="7"/>
@@ -3132,33 +3122,33 @@
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="7"/>
-      <c r="C166" s="6"/>
+      <c r="C166" s="6">
+        <v>6</v>
+      </c>
       <c r="D166" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E166" s="7"/>
-      <c r="F166" s="7"/>
+      <c r="F166" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="7"/>
-      <c r="C167" s="6">
-        <v>8</v>
-      </c>
+      <c r="C167" s="6"/>
       <c r="D167" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E167" s="7"/>
-      <c r="F167" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F167" s="7"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="7"/>
       <c r="C168" s="6"/>
       <c r="D168" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E168" s="7"/>
       <c r="F168" s="7"/>
@@ -3166,33 +3156,33 @@
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="7"/>
-      <c r="C169" s="6"/>
+      <c r="C169" s="6">
+        <v>7</v>
+      </c>
       <c r="D169" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E169" s="7"/>
-      <c r="F169" s="7"/>
+      <c r="F169" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="7"/>
-      <c r="C170" s="6">
-        <v>9</v>
-      </c>
+      <c r="C170" s="6"/>
       <c r="D170" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E170" s="7"/>
-      <c r="F170" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F170" s="7"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="7"/>
       <c r="C171" s="6"/>
       <c r="D171" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E171" s="7"/>
       <c r="F171" s="7"/>
@@ -3200,33 +3190,33 @@
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="7"/>
-      <c r="C172" s="6"/>
+      <c r="C172" s="6">
+        <v>8</v>
+      </c>
       <c r="D172" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E172" s="7"/>
-      <c r="F172" s="7"/>
+      <c r="F172" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="7"/>
-      <c r="C173" s="6">
-        <v>10</v>
-      </c>
+      <c r="C173" s="6"/>
       <c r="D173" s="7" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="E173" s="7"/>
-      <c r="F173" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="F173" s="7"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="7"/>
       <c r="C174" s="6"/>
       <c r="D174" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E174" s="7"/>
       <c r="F174" s="7"/>
@@ -3234,27 +3224,85 @@
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="7"/>
-      <c r="C175" s="6"/>
+      <c r="C175" s="6">
+        <v>9</v>
+      </c>
       <c r="D175" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E175" s="7"/>
-      <c r="F175" s="7"/>
+      <c r="F175" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="7"/>
-      <c r="C176" s="6">
-        <v>11</v>
-      </c>
+      <c r="C176" s="6"/>
       <c r="D176" s="7" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="E176" s="7"/>
       <c r="F176" s="7"/>
     </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="4"/>
+      <c r="B177" s="7"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="4"/>
+      <c r="B178" s="7"/>
+      <c r="C178" s="6">
+        <v>10</v>
+      </c>
+      <c r="D178" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E178" s="7"/>
+      <c r="F178" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="4"/>
+      <c r="B179" s="7"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E179" s="7"/>
+      <c r="F179" s="7"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="4"/>
+      <c r="B180" s="7"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E180" s="7"/>
+      <c r="F180" s="7"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="4"/>
+      <c r="B181" s="7"/>
+      <c r="C181" s="6">
+        <v>11</v>
+      </c>
+      <c r="D181" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E181" s="7"/>
+      <c r="F181" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F145"/>
+  <autoFilter ref="A1:F150"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mejoras a las vistas y arreglo de algunos auxiliares
</commit_message>
<xml_diff>
--- a/public/Equipos_Docentes.xlsx
+++ b/public/Equipos_Docentes.xlsx
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="G99" sqref="G99"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>